<commit_message>
EPBDS-9436 Add test for getValue error message for case sensitive case
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-12609_CaseSensitivity_Warnings.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-12609_CaseSensitivity_Warnings.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\sample\user-workspace\DEFAULT\1111111111111111\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\demoMaster\openl-demo\user-workspace\DEFAULT\EPBDS-12609_CaseSensitivity_Warnings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CDCC6A6-0421-4F6E-9764-116851744F31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B315F042-360F-4F3E-BF8B-A7816645F5EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3C8E964E-D9CC-5E4F-871B-4446146234FE}"/>
+    <workbookView xWindow="1200" yWindow="3105" windowWidth="30465" windowHeight="15540" xr2:uid="{3C8E964E-D9CC-5E4F-871B-4446146234FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="55">
   <si>
     <t>String</t>
   </si>
@@ -94,9 +94,6 @@
     <t>=$Values$Step1(mySpr2(a))</t>
   </si>
   <si>
-    <t>=(Integer)mySpr(a).getFieldValue("$Step1")</t>
-  </si>
-  <si>
     <t>Spreadsheet SpreadsheetResult  MySpr3(String[] arr1, String[] arr2, String channel)</t>
   </si>
   <si>
@@ -176,17 +173,40 @@
   </si>
   <si>
     <t>=(Integer)mySprB(a).getFieldValue("$Step1")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datatype StrField &lt;String&gt; </t>
+  </si>
+  <si>
+    <t>aaa</t>
+  </si>
+  <si>
+    <t>bbb</t>
+  </si>
+  <si>
+    <t>ccc</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult mySpr4(MyDatatype param)</t>
+  </si>
+  <si>
+    <t>getValue</t>
+  </si>
+  <si>
+    <t>=getValue(strField)</t>
+  </si>
+  <si>
+    <t>// The case with Case sensitivity  for vocabulary and getValue() method EPBDS-9436</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
-      <color theme="1" rgb="000000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -232,9 +252,9 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,6 +266,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -264,9 +285,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office 2013–2022">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -304,7 +325,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -410,7 +431,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -552,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -560,25 +581,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DCF6AC2-7B92-B044-AECA-1BE367F9ADBC}">
-  <dimension ref="C8:E69"/>
+  <dimension ref="C8:E83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="78.09765625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="32.19921875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.296875" collapsed="false"/>
+    <col min="3" max="3" width="78.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>0</v>
       </c>
@@ -586,12 +607,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="3:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>2</v>
       </c>
@@ -599,7 +620,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>4</v>
       </c>
@@ -607,7 +628,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>7</v>
       </c>
@@ -615,13 +636,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D19" s="6"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="3" t="s">
         <v>2</v>
       </c>
@@ -629,7 +650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="3" t="s">
         <v>10</v>
       </c>
@@ -638,13 +659,13 @@
       </c>
       <c r="E21" s="1"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D23" s="6"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C24" s="3" t="s">
         <v>2</v>
       </c>
@@ -652,7 +673,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
@@ -660,13 +681,13 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="3" t="s">
         <v>2</v>
       </c>
@@ -674,37 +695,37 @@
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="3" t="s">
         <v>15</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
     </row>
-    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="3"/>
     </row>
-    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C36" s="3">
         <v>1</v>
       </c>
@@ -712,10 +733,10 @@
         <v>20</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C37" s="3">
         <v>40</v>
       </c>
@@ -726,7 +747,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C38" s="3">
         <v>50</v>
       </c>
@@ -734,15 +755,15 @@
         <v>60</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="42" spans="3:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="3:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
         <v>2</v>
       </c>
@@ -750,20 +771,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C44" t="s">
         <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="3:5" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="3:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
         <v>2</v>
       </c>
@@ -771,20 +792,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
         <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C54" t="s">
         <v>2</v>
       </c>
@@ -792,36 +813,36 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C55" t="s">
+        <v>25</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D55" s="1" t="s">
+    </row>
+    <row r="56" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="56" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
+      <c r="D56" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="1" t="s">
+    </row>
+    <row r="57" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="57" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
+      <c r="D57" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D57" s="1" t="s">
+    </row>
+    <row r="60" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="60" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="61" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C61" t="s">
         <v>2</v>
       </c>
@@ -829,54 +850,108 @@
         <v>9</v>
       </c>
     </row>
-    <row r="62" spans="3:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C62" t="s">
         <v>4</v>
       </c>
       <c r="D62" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C65" s="3" t="s">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D65" s="3"/>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C66" s="3" t="s">
+      <c r="D66" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D66" s="5" t="s">
+    </row>
+    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C67" s="3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C67" s="3" t="s">
+      <c r="D67" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D67" s="5" t="s">
+    </row>
+    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C68" s="3" t="s">
+      <c r="D68" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D68" s="3" t="s">
+    </row>
+    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C69" s="3" t="s">
+      <c r="D69" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D69" s="5" t="s">
-        <v>42</v>
-      </c>
+    </row>
+    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="74" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D79" s="7"/>
+    </row>
+    <row r="80" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="81" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="82" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D82" s="1"/>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="D83" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="C79:D79"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="C28:D28"/>

</xml_diff>